<commit_message>
some reorganization to calculation
</commit_message>
<xml_diff>
--- a/surg_one_for_one.xlsx
+++ b/surg_one_for_one.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MattC\Documents\repos\inj_matrix\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MattC\Documents\repos\inj_surg_impact\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -110,12 +110,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -130,9 +136,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,7 +423,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -486,10 +493,10 @@
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>0.8</v>
       </c>
       <c r="E4">
@@ -503,10 +510,10 @@
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>0.2</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>0.8</v>
       </c>
       <c r="E5">
@@ -523,7 +530,7 @@
       <c r="C6">
         <v>0.8</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>0.8</v>
       </c>
       <c r="E6">

</xml_diff>